<commit_message>
Chuc nang phan mem
</commit_message>
<xml_diff>
--- a/Documents/ProjectProposal_ChucNangPhanMem.xlsx
+++ b/Documents/ProjectProposal_ChucNangPhanMem.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NMCNPM\trunk\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GocHocTap\HOAN CHINH DAI HOC\Nhap mon cong nghe phan mem\Project\trunk\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2438D602-E8C2-494B-AFAA-504D2F8EC455}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Tên chức năng</t>
   </si>
@@ -59,74 +54,109 @@
     <t>chỉ những user được admin đăng ký mới được sử dụng</t>
   </si>
   <si>
-    <t>Xem danh sách các phạm nhân</t>
+    <t>Chỉ user thuộc bộ phận y tế mới được phép sử dụng</t>
   </si>
   <si>
     <t>Hiển thị danh sách các phạm nhân bao gồm:
 -Họ tên, ngày sinh, địa chỉ của các phạm nhân
--Mức độ phạm tội, tình trạng giam giữ
--Tình trạng sức khỏe, có được gặp người thân hay không</t>
-  </si>
-  <si>
-    <t>Đối với user là người nhà phạm nhân, chỉ được phép xem danh
-sách đã hiển thị sẵn có.
-Đối với user là bộ phận quản giáo, dựa vào mức độ phạm tội và tình trạng sức khỏe của phạm nhân sẽ đưa ra chế độ giám sát phù hợp</t>
-  </si>
-  <si>
-    <t>Khám bệnh</t>
-  </si>
-  <si>
-    <t>Mỗi phạm nhân đều có thông số thể hiện Tình trạng sức khỏe:
--Chức năng cho phép liệt kê danh sách các tù nhân được chăm sóc trong ngày
--Cập nhật tình trạng sức khỏe bệnh nhân, ngày kiểm tra định kì (nếu có),…</t>
-  </si>
-  <si>
-    <t>Chỉ user thuộc bộ phận y tế mới được phép sử dụng</t>
-  </si>
-  <si>
-    <t>Tiếp nhận và phóng thích</t>
-  </si>
-  <si>
-    <t>Chức năng bao gồm:
--Cập nhật danh sách phạm nhân(họ tên, địa chỉ, số điện thoại người thân, tình trạn sức khỏe, mức độ phạm tội, …).
--Xuất danh sách phạm nhân sẽ được tiếp nhận và phạm nhân phóng thích trong ngày, trong tháng, trong năm.
--Lên lịch thăm nuôi cho thân nhân của phạm nhân</t>
-  </si>
-  <si>
-    <t>Chỉ user thuộc bộ phận này mới được phép sử dụng</t>
-  </si>
-  <si>
-    <t>Cung cấp thức ăn</t>
-  </si>
-  <si>
-    <t>Chức năng dùng để cung cấp khẩu phần ăn và chế độ phù hợp cho cán bộ nhân viên của các bộ phận và các phạm nhân: 
--Xuất danh sách cán bộ nhân viên của các bộ phận, xuất danh sách các phạm nhân để từ đó cung cấp thức ăn từng bữa cho phù hợp.
--Đối với một số phạm nhân có tình trạng đặc biệt theo chỉ định của bộ phận y tế, bộ phận cấp dưỡng sẽ có chế độ dinh dưỡng phù hợp.</t>
-  </si>
-  <si>
-    <t>Quản lý hệ thống</t>
-  </si>
-  <si>
-    <t>Chức năng cho phép quản lý tổng thể tất cả các bộ phận trong hệ thống:
--Xuất ra danh sách các hoạt động theo từng bộ phận 
--Xuất ra danh sách phạm nhân tiếp nhận và phóng thích trong ngày, trong
-tháng
--Liệt kê phạm nhân dựa theo mức độ phạm tội, theo ngày phóng thích
--Phân chia lịch trực của từng bộ phận,...</t>
-  </si>
-  <si>
-    <t>Cải tạo</t>
-  </si>
-  <si>
-    <t>Chịu trác nhiệm cập nhật khả năng, năng khiếu của từng phạm nhân.
--Đề nghị các hoạt động phù hợp với từng phạm nhân
--Cập nhật mức độ cải tạo của từng phạm nhân, đưa ra các đề nghị khen thưởng cho phạm nhân tốt, . . .</t>
+-Mức độ phạm tội
+-Tình trạng giam giữ
+-Tình trạng sức khỏe
+-Có được gặp người thân hay không</t>
+  </si>
+  <si>
+    <t>- Đối với user là người nhà phạm nhân, chỉ được phép xem thông tin liên quan đến người nhà đó (tình trạng giam giữ, tình trạng sức khỏe,...)
+- Đối với user là bộ phận quản giáo, dựa vào mức độ phạm tội và tình trạng sức khỏe của phạm nhân sẽ đưa ra chế độ giám sát phù hợp</t>
+  </si>
+  <si>
+    <t>Cập nhật sức khỏe</t>
+  </si>
+  <si>
+    <t>Cập nhật tình trạng sức khỏe bệnh nhân, ngày kiểm tra định kì (nếu có),…</t>
+  </si>
+  <si>
+    <t>Xem danh sách phạm nhân</t>
+  </si>
+  <si>
+    <t>Thêm mới/Cập nhật phạm nhân</t>
+  </si>
+  <si>
+    <t>Cập nhật/Thêm mới danh sách phạm nhân(họ tên, địa chỉ, số điện thoại người thân, tình trạng sức khỏe, mức độ phạm tội, …).</t>
+  </si>
+  <si>
+    <t>Chỉ user thuộc bộ phận Tiếp nhân&amp;Phóng thích mới được phép sử dụng</t>
+  </si>
+  <si>
+    <t>Xuất danh sách phạm nhân được tiếp nhận &amp; phóng thích</t>
+  </si>
+  <si>
+    <t>Xuất danh sách phạm nhân sẽ được tiếp nhận và phạm nhân phóng thích trong ngày, trong tháng</t>
+  </si>
+  <si>
+    <t>Lên lịch thăm nuôi</t>
+  </si>
+  <si>
+    <t>Lên lịch thăm nuôi cho thân nhân của phạm nhân</t>
+  </si>
+  <si>
+    <t>Cấp dưỡng</t>
+  </si>
+  <si>
+    <t>Xuất danh sách cán bộ nhân viên của các bộ phận, xuất danh sách các phạm nhân cùng tình trạng theo chỉ định của bộ phận y tế của phạm nhân đó</t>
+  </si>
+  <si>
+    <t>Chỉ user thuộc bộ phận cấp dưỡng mới được phép sử dụng</t>
+  </si>
+  <si>
+    <t>Chỉ user thuộc Bộ phận Tiếp nhân&amp;Phóng thích và Bộ phận Quản lý mới được phép sử dụng</t>
+  </si>
+  <si>
+    <t>Xuất danh sách hoạt động của các bộ phận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xuất ra danh sách các hoạt động theo từng bộ phận </t>
+  </si>
+  <si>
+    <t>Liệt kê phạm nhân</t>
+  </si>
+  <si>
+    <t>Chỉ user thuộc Bộ phận y tế và Bộ phận quản lý mới được phép sử dụng</t>
+  </si>
+  <si>
+    <t>Liệt kê phạm nhân theo các tiêu chí cụ thể (hiển thị theo chức năng xem danh sách phạm nhân):
+- Theo chế độ chăm sóc trong ngày
+- Mức độ phạm tội
+- Ngày phóng thích</t>
+  </si>
+  <si>
+    <t>Chỉ user thuộc Bộ phận quản lý mới được phép sử dụng</t>
+  </si>
+  <si>
+    <t>Cập nhật khả năng/năng khiếu phạm nhân</t>
+  </si>
+  <si>
+    <t>Chỉ user thuộc bộ phận Cải tạo mới được phép sử dụng</t>
+  </si>
+  <si>
+    <t>Cập nhật mức độ cải tạo phạm nhân</t>
+  </si>
+  <si>
+    <t>Cập nhật mức độ cải tạo của từng phạm nhân</t>
+  </si>
+  <si>
+    <t>Xuất đề nghị khen thưởng</t>
+  </si>
+  <si>
+    <t>Đưa ra các đề nghị khen thưởng cho phạm nhân tốt</t>
+  </si>
+  <si>
+    <t>Cập nhật khả năng, năng khiếu của từng phạm nhân, đề nghị hoạt động phù hợp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -186,16 +216,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,117 +540,170 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="58.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="65.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bang Nhan Su & Chi Phi cua du an - Muc 5, Temp#0
</commit_message>
<xml_diff>
--- a/Documents/ProjectProposal_ChucNangPhanMem.xlsx
+++ b/Documents/ProjectProposal_ChucNangPhanMem.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GocHocTap\HOAN CHINH DAI HOC\Nhap mon cong nghe phan mem\Project\trunk\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NMCNPM\trunk\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2438D602-E8C2-494B-AFAA-504D2F8EC455}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +83,6 @@
     <t>Cập nhật/Thêm mới danh sách phạm nhân(họ tên, địa chỉ, số điện thoại người thân, tình trạng sức khỏe, mức độ phạm tội, …).</t>
   </si>
   <si>
-    <t>Chỉ user thuộc bộ phận Tiếp nhân&amp;Phóng thích mới được phép sử dụng</t>
-  </si>
-  <si>
     <t>Xuất danh sách phạm nhân được tiếp nhận &amp; phóng thích</t>
   </si>
   <si>
@@ -106,9 +102,6 @@
   </si>
   <si>
     <t>Chỉ user thuộc bộ phận cấp dưỡng mới được phép sử dụng</t>
-  </si>
-  <si>
-    <t>Chỉ user thuộc Bộ phận Tiếp nhân&amp;Phóng thích và Bộ phận Quản lý mới được phép sử dụng</t>
   </si>
   <si>
     <t>Xuất danh sách hoạt động của các bộ phận</t>
@@ -152,11 +145,17 @@
   <si>
     <t>Cập nhật khả năng, năng khiếu của từng phạm nhân, đề nghị hoạt động phù hợp</t>
   </si>
+  <si>
+    <t>Chỉ user thuộc bộ phận Tiếp nhận&amp;Phóng thích mới được phép sử dụng</t>
+  </si>
+  <si>
+    <t>Chỉ user thuộc Bộ phận Tiếp nhận&amp;Phóng thích và Bộ phận Quản lý mới được phép sử dụng</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -540,10 +539,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -615,95 +616,95 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mockup - ios android
</commit_message>
<xml_diff>
--- a/Documents/ProjectProposal_ChucNangPhanMem.xlsx
+++ b/Documents/ProjectProposal_ChucNangPhanMem.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NMCNPM\trunk\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GocHocTap\HOAN CHINH DAI HOC\Nhap mon cong nghe phan mem\Project\trunk\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6D6145-2778-4465-9E5D-E60AF0705097}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -206,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -217,14 +218,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,28 +549,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="65.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -568,10 +576,10 @@
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -579,10 +587,10 @@
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -590,10 +598,10 @@
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -601,10 +609,10 @@
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -612,10 +620,10 @@
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -623,10 +631,10 @@
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -634,10 +642,10 @@
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -645,10 +653,10 @@
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -656,10 +664,10 @@
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -667,10 +675,10 @@
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -678,10 +686,10 @@
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -689,10 +697,10 @@
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -700,10 +708,10 @@
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="8" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>